<commit_message>
added organize gi src 2
</commit_message>
<xml_diff>
--- a/Excel_files/GI_tables/GI_Src_2.xlsx
+++ b/Excel_files/GI_tables/GI_Src_2.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="989" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="990" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="PDFTables.com" sheetId="1" state="visible" r:id="rId2"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8795" uniqueCount="3023">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8794" uniqueCount="3022">
   <si>
     <t xml:space="preserve">food number</t>
   </si>
@@ -9086,9 +9086,6 @@
   </si>
   <si>
     <t xml:space="preserve"> White yam, peeled, cubed, boiled 30 min (Jamaica)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">(Jamaica)</t>
   </si>
 </sst>
 </file>
@@ -9218,20 +9215,20 @@
   </sheetPr>
   <dimension ref="A1:I65536"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A2" activeCellId="0" sqref="A2"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2431" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A2454" activeCellId="0" sqref="A2454"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="70.4858299595142"/>
-    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="198.17004048583"/>
+    <col collapsed="false" hidden="false" max="1" min="1" style="1" width="7.48987854251012"/>
+    <col collapsed="false" hidden="false" max="2" min="2" style="1" width="199.991902834008"/>
     <col collapsed="false" hidden="false" max="3" min="3" style="1" width="8.67611336032389"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="18.9595141700405"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="1" width="19.1740890688259"/>
     <col collapsed="false" hidden="false" max="5" min="5" style="1" width="16.3886639676113"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="16.1740890688259"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="1" width="16.2834008097166"/>
     <col collapsed="false" hidden="false" max="7" min="7" style="1" width="9"/>
-    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="22.3886639676113"/>
+    <col collapsed="false" hidden="false" max="8" min="8" style="1" width="22.4939271255061"/>
     <col collapsed="false" hidden="false" max="9" min="9" style="1" width="16.3886639676113"/>
     <col collapsed="false" hidden="false" max="1025" min="10" style="0" width="8.57085020242915"/>
   </cols>
@@ -70874,55 +70871,41 @@
       </c>
     </row>
     <row r="2454" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2454" s="0"/>
-      <c r="B2454" s="4" t="s">
-        <v>3022</v>
-      </c>
-      <c r="C2454" s="0"/>
-      <c r="D2454" s="0"/>
-      <c r="E2454" s="0"/>
-      <c r="F2454" s="0"/>
-      <c r="G2454" s="0"/>
-      <c r="H2454" s="0"/>
       <c r="I2454" s="3" t="n">
-        <v>28</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2455" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="I2455" s="3" t="n">
-        <v>23</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2456" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="I2456" s="3" t="n">
-        <v>32</v>
+        <v>20</v>
       </c>
     </row>
     <row r="2457" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="I2457" s="3" t="n">
-        <v>20</v>
+        <v>32</v>
       </c>
     </row>
     <row r="2458" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="I2458" s="3" t="n">
-        <v>32</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2459" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="I2459" s="3" t="n">
-        <v>15</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2460" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="I2460" s="3" t="n">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="2461" customFormat="false" ht="14.25" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="I2461" s="3" t="n">
         <v>28</v>
       </c>
     </row>
+    <row r="1048575" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <mergeCells count="48">

</xml_diff>